<commit_message>
Working Backend-functionality Draft-I Feb 28th 2020
</commit_message>
<xml_diff>
--- a/Application Metadata/FI_Activity_Tracker.xlsx
+++ b/Application Metadata/FI_Activity_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FA8788-D8D6-4B41-8252-688B2A88A42A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D67337-CE32-4372-99A3-49B15292B83C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,18 @@
   <si>
     <t>Successfully displayed nested hierarchical set of XSD Tags.
 Worked on creating final dataframe logic and successfully managed to create Pyspark config.csv file as per discussion with Pooja.</t>
+  </si>
+  <si>
+    <t>Finalizing Draft 1 of working application</t>
+  </si>
+  <si>
+    <t>Updated doc-strings, updated input form for destination-file seperator, and ensured navigations working properly after login</t>
+  </si>
+  <si>
+    <t>Excel file with Pooja's specific requirements</t>
+  </si>
+  <si>
+    <t>Created the precise config excel file containing format as required</t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -269,11 +281,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,9 +333,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -307,50 +342,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,17 +688,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" style="12" customWidth="1"/>
     <col min="4" max="4" width="63.453125" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
@@ -669,36 +725,36 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
+      <c r="A2" s="13">
         <v>43855</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="14">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="23">
         <v>0.4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="15">
+      <c r="A3" s="13">
         <v>43856</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="14">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="9">
+      <c r="C3" s="20"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="14">
         <v>8</v>
       </c>
     </row>
@@ -706,19 +762,19 @@
       <c r="A4" s="8">
         <v>43860</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>0.5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>3</v>
       </c>
     </row>
@@ -726,51 +782,51 @@
       <c r="A5" s="8">
         <v>43861</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>0.5</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="15">
+      <c r="A6" s="13">
         <v>43862</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="25">
         <v>3</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>0.4</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>43863</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>0.6</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>12</v>
       </c>
     </row>
@@ -778,17 +834,17 @@
       <c r="A8" s="8">
         <v>43864</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12">
+      <c r="C8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11">
         <v>0</v>
       </c>
     </row>
@@ -796,17 +852,17 @@
       <c r="A9" s="8">
         <v>43865</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="14">
         <v>5</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="12">
+      <c r="E9" s="9"/>
+      <c r="F9" s="11">
         <v>2</v>
       </c>
     </row>
@@ -814,17 +870,17 @@
       <c r="A10" s="8">
         <v>43866</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="14">
         <v>6</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12">
+      <c r="C10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11">
         <v>0</v>
       </c>
     </row>
@@ -832,19 +888,19 @@
       <c r="A11" s="8">
         <v>43867</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="14">
         <v>7</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>0.05</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="11">
         <v>2</v>
       </c>
     </row>
@@ -852,53 +908,53 @@
       <c r="A12" s="8">
         <v>43868</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="14">
         <v>8</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="10">
         <v>0.1</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>43869</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="14">
         <v>9</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <v>0.1</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>43870</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="14">
         <v>10</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <v>0.4</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>9</v>
       </c>
     </row>
@@ -906,17 +962,17 @@
       <c r="A15" s="8">
         <v>43871</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="14">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12">
+      <c r="E15" s="9"/>
+      <c r="F15" s="11">
         <v>0</v>
       </c>
     </row>
@@ -924,19 +980,19 @@
       <c r="A16" s="8">
         <v>43872</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="14">
         <v>12</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>0.4</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>3</v>
       </c>
     </row>
@@ -944,17 +1000,17 @@
       <c r="A17" s="8">
         <v>43873</v>
       </c>
-      <c r="B17" s="9">
-        <v>13</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12">
+      <c r="B17" s="14">
+        <v>13</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11">
         <v>0</v>
       </c>
     </row>
@@ -962,17 +1018,17 @@
       <c r="A18" s="8">
         <v>43874</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="14">
         <v>14</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="12">
+      <c r="C18" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11">
         <v>0</v>
       </c>
     </row>
@@ -980,71 +1036,385 @@
       <c r="A19" s="8">
         <v>43875</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="14">
         <v>15</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <v>0.1</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="15">
+      <c r="A20" s="13">
         <v>43876</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="14">
         <v>16</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>0.7</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="11">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="13">
         <v>43877</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="12"/>
+      <c r="B21" s="14">
+        <v>17</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>43878</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="12"/>
+      <c r="B22" s="14">
+        <v>18</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="28"/>
+      <c r="F22" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
         <v>43879</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="12"/>
+      <c r="B23" s="14">
+        <v>19</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="28"/>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="8">
+        <v>43880</v>
+      </c>
+      <c r="B24" s="14">
+        <v>20</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>43881</v>
+      </c>
+      <c r="B25" s="14">
+        <v>21</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="8">
+        <v>43882</v>
+      </c>
+      <c r="B26" s="14">
+        <v>22</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="13">
+        <v>43883</v>
+      </c>
+      <c r="B27" s="14">
+        <v>23</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="13">
+        <v>43884</v>
+      </c>
+      <c r="B28" s="14">
+        <v>24</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="8">
+        <v>43885</v>
+      </c>
+      <c r="B29" s="14">
+        <v>25</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>43886</v>
+      </c>
+      <c r="B30" s="14">
+        <v>26</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>43887</v>
+      </c>
+      <c r="B31" s="14">
+        <v>27</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="8">
+        <v>43888</v>
+      </c>
+      <c r="B32" s="14">
+        <v>28</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="8">
+        <v>43889</v>
+      </c>
+      <c r="B33" s="14">
+        <v>29</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="13">
+        <v>43890</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="13">
+        <v>43891</v>
+      </c>
+      <c r="B35" s="33"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="8">
+        <v>43892</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="8">
+        <v>43893</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="8">
+        <v>43894</v>
+      </c>
+      <c r="B38" s="33"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="8">
+        <v>43895</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="8">
+        <v>43896</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="13">
+        <v>43897</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="13">
+        <v>43898</v>
+      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="8">
+        <v>43899</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="8">
+        <v>43900</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="32"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="8">
+        <v>43901</v>
+      </c>
+      <c r="B45" s="33"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="8">
+        <v>43902</v>
+      </c>
+      <c r="B46" s="33"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="32"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="8">
+        <v>43903</v>
+      </c>
+      <c r="B47" s="33"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F23" xr:uid="{56211E31-1F8D-4D32-83EF-276A8FFA7390}"/>

</xml_diff>